<commit_message>
Updated pie charts to show team names instead of abbreviations
</commit_message>
<xml_diff>
--- a/2022MLR/Weekly Forecasts/Round_8.xlsx
+++ b/2022MLR/Weekly Forecasts/Round_8.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RugbyPredictifier\2022MLR\Weekly Forecasts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{8AB7148C-543D-4BDA-A5FF-015314184A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Round 8" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="43">
   <si>
     <t>City</t>
   </si>
@@ -155,14 +148,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#0%"/>
     <numFmt numFmtId="167" formatCode="#0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,17 +366,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -391,14 +384,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -445,7 +430,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,27 +462,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -529,24 +496,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -722,7 +671,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -730,16 +679,9 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.44140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:61">
       <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
@@ -789,913 +731,1213 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:61">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="H2" s="14" t="s">
+      <c r="F2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="K2" s="14" t="s">
+      <c r="I2" s="12"/>
+      <c r="K2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="N2" s="14" t="s">
+      <c r="L2" s="12"/>
+      <c r="N2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="14"/>
-    </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:61">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15">
-        <v>0.19745571026000761</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="E3" s="15">
-        <v>0.70693130792250036</v>
-      </c>
-      <c r="F3" s="15"/>
-      <c r="H3" s="15">
-        <v>0.63667612936896745</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="K3" s="15">
-        <v>0.62203319624932796</v>
-      </c>
-      <c r="L3" s="15"/>
-      <c r="N3" s="15">
-        <v>0.52545724326458543</v>
-      </c>
-      <c r="O3" s="15"/>
-    </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B3" s="13">
+        <v>0.1974557102600076</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="E3" s="13">
+        <v>0.7069313079225004</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="H3" s="13">
+        <v>0.6366761293689674</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="K3" s="13">
+        <v>0.622033196249328</v>
+      </c>
+      <c r="L3" s="13"/>
+      <c r="N3" s="13">
+        <v>0.5254572432645854</v>
+      </c>
+      <c r="O3" s="13"/>
+    </row>
+    <row r="4" spans="1:61">
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15">
-        <v>0.1739651855483535</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="E4" s="15">
-        <v>0.98176908823673248</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="H4" s="15">
-        <v>0.94637023577372581</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="K4" s="15">
-        <v>0.83595328186158158</v>
-      </c>
-      <c r="L4" s="15"/>
-      <c r="N4" s="15">
-        <v>0.57061442725206923</v>
-      </c>
-      <c r="O4" s="15"/>
-    </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B4" s="13">
+        <v>0.1741601265967204</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="E4" s="13">
+        <v>0.9817892523784408</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="H4" s="13">
+        <v>0.9464219349638932</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="K4" s="13">
+        <v>0.8355359226171654</v>
+      </c>
+      <c r="L4" s="13"/>
+      <c r="N4" s="13">
+        <v>0.570921723994494</v>
+      </c>
+      <c r="O4" s="13"/>
+    </row>
+    <row r="5" spans="1:61">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14">
-        <v>3.4350419272964152</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="E5" s="14">
-        <v>69.404330562507397</v>
-      </c>
-      <c r="F5" s="14"/>
-      <c r="H5" s="14">
-        <v>60.253133866241278</v>
-      </c>
-      <c r="I5" s="14"/>
-      <c r="K5" s="14">
-        <v>51.999069183147498</v>
-      </c>
-      <c r="L5" s="14"/>
-      <c r="N5" s="14">
-        <v>29.983348391087262</v>
-      </c>
-      <c r="O5" s="14"/>
-    </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B5" s="12">
+        <v>3.438891149612826</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="E5" s="12">
+        <v>69.40575602881449</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="H5" s="12">
+        <v>60.25642543027001</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="K5" s="12">
+        <v>51.97310805266865</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="N5" s="12">
+        <v>29.99949552100113</v>
+      </c>
+      <c r="O5" s="12"/>
+    </row>
+    <row r="6" spans="1:61">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
-        <v>2.5800799999999999E-2</v>
-      </c>
-      <c r="C6" s="12">
-        <v>0.96618680000000001</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0.5476162</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0.3976576</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0.61342399999999997</v>
-      </c>
-      <c r="I6" s="12">
-        <v>0.35186640000000002</v>
-      </c>
-      <c r="K6" s="12">
-        <v>0.70303660000000001</v>
-      </c>
-      <c r="L6" s="12">
-        <v>0.25503500000000001</v>
-      </c>
-      <c r="N6" s="12">
-        <v>0.84415600000000002</v>
-      </c>
-      <c r="O6" s="12">
-        <v>0.1315876</v>
-      </c>
-    </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B6" s="14">
+        <v>0.0258388</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.966187</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.5476224</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.3977334</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.613217</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.3518456</v>
+      </c>
+      <c r="K6" s="14">
+        <v>0.7033068</v>
+      </c>
+      <c r="L6" s="14">
+        <v>0.2547608</v>
+      </c>
+      <c r="N6" s="14">
+        <v>0.8440182000000001</v>
+      </c>
+      <c r="O6" s="14">
+        <v>0.1316954</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13">
-        <v>14.9772088</v>
-      </c>
-      <c r="C7" s="13">
-        <v>32.171084</v>
-      </c>
-      <c r="E7" s="13">
-        <v>26.238949600000002</v>
-      </c>
-      <c r="F7" s="13">
-        <v>24.538862200000001</v>
-      </c>
-      <c r="H7" s="13">
-        <v>17.908712999999999</v>
-      </c>
-      <c r="I7" s="13">
-        <v>14.968705399999999</v>
-      </c>
-      <c r="K7" s="13">
-        <v>26.408078799999998</v>
-      </c>
-      <c r="L7" s="13">
-        <v>20.686098399999999</v>
-      </c>
-      <c r="N7" s="13">
-        <v>25.814344200000001</v>
-      </c>
-      <c r="O7" s="13">
-        <v>14.789289</v>
-      </c>
-    </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="B7" s="15">
+        <v>14.9748266</v>
+      </c>
+      <c r="C7" s="15">
+        <v>32.1647276</v>
+      </c>
+      <c r="E7" s="15">
+        <v>26.236637</v>
+      </c>
+      <c r="F7" s="15">
+        <v>24.535916</v>
+      </c>
+      <c r="H7" s="15">
+        <v>17.9065702</v>
+      </c>
+      <c r="I7" s="15">
+        <v>14.9645436</v>
+      </c>
+      <c r="K7" s="15">
+        <v>26.4110108</v>
+      </c>
+      <c r="L7" s="15">
+        <v>20.6831026</v>
+      </c>
+      <c r="N7" s="15">
+        <v>25.8072074</v>
+      </c>
+      <c r="O7" s="15">
+        <v>14.7826506</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="15">
         <v>7</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="15">
         <v>20</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="15">
         <v>15</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="15">
         <v>14</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="15">
         <v>9</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="15">
         <v>3</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="15">
         <v>14</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="15">
         <v>10</v>
       </c>
-      <c r="N8" s="13">
-        <v>15</v>
-      </c>
-      <c r="O8" s="13">
+      <c r="N8" s="15">
+        <v>14</v>
+      </c>
+      <c r="O8" s="15">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:61">
       <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="15">
         <v>8</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="15">
         <v>23</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="15">
         <v>17</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="15">
         <v>17</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="15">
         <v>11</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="15">
         <v>5</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="15">
         <v>17</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="15">
         <v>12</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="15">
         <v>17</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="15">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:61">
       <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="15">
         <v>10</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="15">
         <v>25</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="15">
         <v>20</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="15">
         <v>17</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="15">
         <v>13</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="15">
         <v>7</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="15">
         <v>19</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="15">
         <v>14</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="15">
         <v>19</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="15">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:61">
       <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="15">
         <v>10</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="15">
         <v>26</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="15">
         <v>21</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="15">
         <v>19</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="15">
         <v>13</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="15">
         <v>7</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="15">
         <v>20</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="15">
         <v>15</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="15">
         <v>20</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="15">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:61">
       <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="15">
         <v>12</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="15">
         <v>27</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="15">
         <v>22</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="15">
         <v>21</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="15">
         <v>14</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="15">
         <v>10</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="15">
         <v>22</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="15">
         <v>17</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="15">
         <v>22</v>
       </c>
-      <c r="O12" s="13">
+      <c r="O12" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:61">
       <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="15">
         <v>12</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="15">
         <v>28</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="15">
         <v>23</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="15">
         <v>22</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="15">
         <v>16</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="15">
         <v>10</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="15">
         <v>22</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="15">
         <v>17</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="15">
         <v>22</v>
       </c>
-      <c r="O13" s="13">
+      <c r="O13" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:61">
       <c r="A14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="15">
         <v>13</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="15">
         <v>30</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="15">
         <v>24</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="15">
         <v>22</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="15">
         <v>16</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="15">
         <v>12</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="15">
         <v>24</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="15">
         <v>19</v>
       </c>
-      <c r="N14" s="13">
+      <c r="N14" s="15">
         <v>24</v>
       </c>
-      <c r="O14" s="13">
+      <c r="O14" s="15">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:61">
       <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="15">
         <v>14</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="15">
         <v>30</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="15">
         <v>25</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="15">
         <v>24</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="15">
         <v>16</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="15">
         <v>13</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="15">
         <v>25</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="15">
         <v>19</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="15">
         <v>24</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:61">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="15">
         <v>15</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="15">
         <v>32</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="15">
         <v>26</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="15">
         <v>24</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="15">
         <v>17</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="15">
         <v>14</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="15">
         <v>26</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="15">
         <v>19</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="15">
         <v>25</v>
       </c>
-      <c r="O16" s="13">
+      <c r="O16" s="15">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15">
       <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="15">
         <v>15</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="15">
         <v>32</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="15">
         <v>27</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="15">
         <v>24</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="15">
         <v>18</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="15">
         <v>14</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="15">
         <v>27</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="15">
         <v>21</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="15">
         <v>26</v>
       </c>
-      <c r="O17" s="13">
+      <c r="O17" s="15">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="15">
         <v>15</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="15">
         <v>33</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="15">
         <v>27</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="15">
         <v>26</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="15">
         <v>19</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="15">
         <v>15</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="15">
         <v>28</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="15">
         <v>22</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="15">
         <v>27</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O18" s="15">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15">
       <c r="A19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="15">
         <v>16</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="15">
         <v>34</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="15">
         <v>28</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="15">
         <v>27</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="15">
         <v>20</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="15">
         <v>17</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K19" s="15">
         <v>29</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="15">
         <v>22</v>
       </c>
-      <c r="N19" s="13">
+      <c r="N19" s="15">
         <v>28</v>
       </c>
-      <c r="O19" s="13">
+      <c r="O19" s="15">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15">
       <c r="A20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="15">
         <v>17</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="15">
         <v>35</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="15">
         <v>29</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="15">
         <v>28</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="15">
         <v>21</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="15">
         <v>17</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="15">
         <v>29</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="15">
         <v>24</v>
       </c>
-      <c r="N20" s="13">
+      <c r="N20" s="15">
         <v>29</v>
       </c>
-      <c r="O20" s="13">
+      <c r="O20" s="15">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15">
       <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="15">
         <v>18</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="15">
         <v>36</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="15">
         <v>30</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="15">
         <v>29</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="15">
         <v>21</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="15">
         <v>19</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="15">
         <v>31</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="15">
         <v>24</v>
       </c>
-      <c r="N21" s="13">
+      <c r="N21" s="15">
         <v>30</v>
       </c>
-      <c r="O21" s="13">
+      <c r="O21" s="15">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15">
       <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="15">
         <v>18</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="15">
         <v>37</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="15">
         <v>31</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="15">
         <v>29</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="15">
         <v>21</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="15">
         <v>20</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="15">
         <v>31</v>
       </c>
-      <c r="L22" s="13">
+      <c r="L22" s="15">
         <v>26</v>
       </c>
-      <c r="N22" s="13">
+      <c r="N22" s="15">
         <v>31</v>
       </c>
-      <c r="O22" s="13">
+      <c r="O22" s="15">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15">
       <c r="A23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="15">
         <v>20</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="15">
         <v>38</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="15">
         <v>32</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="15">
         <v>29</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="15">
         <v>23</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="15">
         <v>21</v>
       </c>
-      <c r="K23" s="13">
+      <c r="K23" s="15">
         <v>33</v>
       </c>
-      <c r="L23" s="13">
+      <c r="L23" s="15">
         <v>26</v>
       </c>
-      <c r="N23" s="13">
+      <c r="N23" s="15">
         <v>32</v>
       </c>
-      <c r="O23" s="13">
+      <c r="O23" s="15">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15">
       <c r="A24" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="15">
         <v>20</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="15">
         <v>40</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="15">
         <v>32</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="15">
         <v>31</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="15">
         <v>23</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="15">
         <v>23</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="15">
         <v>34</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="15">
         <v>27</v>
       </c>
-      <c r="N24" s="13">
+      <c r="N24" s="15">
         <v>33</v>
       </c>
-      <c r="O24" s="13">
+      <c r="O24" s="15">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15">
       <c r="A25" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="15">
         <v>22</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="15">
         <v>41</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="15">
         <v>34</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="15">
         <v>31</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="15">
         <v>24</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="15">
         <v>25</v>
       </c>
-      <c r="K25" s="13">
+      <c r="K25" s="15">
         <v>36</v>
       </c>
-      <c r="L25" s="13">
+      <c r="L25" s="15">
         <v>29</v>
       </c>
-      <c r="N25" s="13">
+      <c r="N25" s="15">
         <v>34</v>
       </c>
-      <c r="O25" s="13">
+      <c r="O25" s="15">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15">
       <c r="A26" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="15">
         <v>24</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="15">
         <v>44</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="15">
         <v>36</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="15">
         <v>36</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="15">
         <v>26</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="15">
         <v>28</v>
       </c>
-      <c r="K26" s="13">
+      <c r="K26" s="15">
         <v>38</v>
       </c>
-      <c r="L26" s="13">
+      <c r="L26" s="15">
         <v>31</v>
       </c>
-      <c r="N26" s="13">
+      <c r="N26" s="15">
         <v>36</v>
       </c>
-      <c r="O26" s="13">
+      <c r="O26" s="15">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15">
       <c r="A27" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="12">
-        <v>3.8399999999999998E-5</v>
-      </c>
-      <c r="C27" s="12">
-        <v>0.54715939999999996</v>
-      </c>
-      <c r="E27" s="12">
-        <v>2.33966E-2</v>
-      </c>
-      <c r="F27" s="12">
-        <v>2.19594E-2</v>
-      </c>
-      <c r="H27" s="12">
-        <v>6.2437999999999999E-3</v>
-      </c>
-      <c r="I27" s="12">
-        <v>4.3089000000000002E-2</v>
-      </c>
-      <c r="K27" s="12">
-        <v>5.1709999999999999E-2</v>
-      </c>
-      <c r="L27" s="12">
-        <v>2.1340999999999999E-2</v>
-      </c>
-      <c r="N27" s="12">
-        <v>0.40799259999999998</v>
-      </c>
-      <c r="O27" s="12">
-        <v>2.2225999999999999E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B27" s="14">
+        <v>4.1e-05</v>
+      </c>
+      <c r="C27" s="14">
+        <v>0.5468836</v>
+      </c>
+      <c r="E27" s="14">
+        <v>0.0233906</v>
+      </c>
+      <c r="F27" s="14">
+        <v>0.0220712</v>
+      </c>
+      <c r="H27" s="14">
+        <v>0.0063</v>
+      </c>
+      <c r="I27" s="14">
+        <v>0.0430286</v>
+      </c>
+      <c r="K27" s="14">
+        <v>0.0516352</v>
+      </c>
+      <c r="L27" s="14">
+        <v>0.0212786</v>
+      </c>
+      <c r="N27" s="14">
+        <v>0.408684</v>
+      </c>
+      <c r="O27" s="14">
+        <v>0.0022236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="12">
-        <v>0.1055812</v>
-      </c>
-      <c r="C28" s="12">
-        <v>2.2291800000000001E-2</v>
-      </c>
-      <c r="E28" s="12">
-        <v>0.246999</v>
-      </c>
-      <c r="F28" s="12">
-        <v>0.28839959999999998</v>
-      </c>
-      <c r="H28" s="12">
-        <v>0.2151168</v>
-      </c>
-      <c r="I28" s="12">
-        <v>0.29016579999999997</v>
-      </c>
-      <c r="K28" s="12">
-        <v>0.17033960000000001</v>
-      </c>
-      <c r="L28" s="12">
-        <v>0.27332240000000002</v>
-      </c>
-      <c r="N28" s="12">
-        <v>8.9923000000000003E-2</v>
-      </c>
-      <c r="O28" s="12">
-        <v>0.1997826</v>
+      <c r="B28" s="14">
+        <v>0.105602</v>
+      </c>
+      <c r="C28" s="14">
+        <v>0.0223064</v>
+      </c>
+      <c r="E28" s="14">
+        <v>0.247284</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0.2883926</v>
+      </c>
+      <c r="H28" s="14">
+        <v>0.2152328</v>
+      </c>
+      <c r="I28" s="14">
+        <v>0.2898912</v>
+      </c>
+      <c r="K28" s="14">
+        <v>0.1701398</v>
+      </c>
+      <c r="L28" s="14">
+        <v>0.2734724</v>
+      </c>
+      <c r="N28" s="14">
+        <v>0.0899042</v>
+      </c>
+      <c r="O28" s="14">
+        <v>0.199789</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="380">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
@@ -1704,18 +1946,78 @@
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="N5:O5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>